<commit_message>
more often evan for bigger n_steps
</commit_message>
<xml_diff>
--- a/python/training_logs.xlsx
+++ b/python/training_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\workspace_masterarbeit\carsim_no_mlagents\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1037A2-207E-46AC-B4F2-221ACAC5C54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15391AA5-4F45-4D90-8928-38757FB4A320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4DC23B-5923-4FA6-B608-7D9F8BF1AED5}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,6 +757,9 @@
       <c r="K3">
         <v>256</v>
       </c>
+      <c r="L3">
+        <v>2800000</v>
+      </c>
       <c r="M3" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
more configs for next test
</commit_message>
<xml_diff>
--- a/python/training_logs.xlsx
+++ b/python/training_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\workspace_masterarbeit\carsim_no_mlagents\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15391AA5-4F45-4D90-8928-38757FB4A320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8557AB-0C5F-4251-A66B-1A4258291888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4DC23B-5923-4FA6-B608-7D9F8BF1AED5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -185,6 +185,81 @@
   </si>
   <si>
     <t>1.7 days</t>
+  </si>
+  <si>
+    <t>medium_standard_distance_reward_only_more_nsteps</t>
+  </si>
+  <si>
+    <t>Lesson</t>
+  </si>
+  <si>
+    <t>3.4 days</t>
+  </si>
+  <si>
+    <t>0.766</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.716</t>
+  </si>
+  <si>
+    <t>-training looks a bit more stable (rollout success_rates do not jump as much)
+-more n_steps do not help in training results
+-slower learning than with less n_steps (less NN updates in the same wall time)</t>
+  </si>
+  <si>
+    <t>medium_standard_ev-velo_reward_resetUponCollision_increasePositiveEventRewards</t>
+  </si>
+  <si>
+    <t>22 h</t>
+  </si>
+  <si>
+    <t>resetUponCollision</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>0.205</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>-agent did not move well
+-agent did not learn to avoid collisions (collision + instantReset means a collision is just as negative as a timeout)</t>
+  </si>
+  <si>
+    <t>-resetUponCollision does not lead to good results in combination with event+velocity reward</t>
+  </si>
+  <si>
+    <t>medium_standard_ev-velo_reward_resetUponCollision_likeMaximilian</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>21h</t>
+  </si>
+  <si>
+    <t>-no agent movement</t>
+  </si>
+  <si>
+    <t>'-resetUponCollision does not lead to good results in combination with event+velocity reward</t>
+  </si>
+  <si>
+    <t>-does resetUponCollision work well with distance reward only?</t>
+  </si>
+  <si>
+    <t>hard standard distance reward only noResetCollision</t>
+  </si>
+  <si>
+    <t>medium_standard distanc_only  resetUponCollision …. In progress</t>
   </si>
 </sst>
 </file>
@@ -220,12 +295,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -540,18 +617,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C51CB6F-A2B2-448C-9258-B2680A9692D9}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="48" customWidth="1"/>
     <col min="16" max="16" width="30.85546875" customWidth="1"/>
+    <col min="29" max="29" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -636,8 +717,11 @@
       <c r="AB1" t="s">
         <v>25</v>
       </c>
+      <c r="AC1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -723,7 +807,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="195" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -807,6 +891,298 @@
       </c>
       <c r="AB3" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="345" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45413</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>64</v>
+      </c>
+      <c r="K4">
+        <v>1024</v>
+      </c>
+      <c r="L4">
+        <v>4600000</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <v>2048</v>
+      </c>
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45414</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>64</v>
+      </c>
+      <c r="K5">
+        <v>256</v>
+      </c>
+      <c r="L5" s="4">
+        <v>45353</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>2048</v>
+      </c>
+      <c r="P5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45415</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>64</v>
+      </c>
+      <c r="K6">
+        <v>64</v>
+      </c>
+      <c r="L6">
+        <v>1700000</v>
+      </c>
+      <c r="M6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6">
+        <v>2048</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45416</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
log success_rate during rollout collection
</commit_message>
<xml_diff>
--- a/python/training_logs.xlsx
+++ b/python/training_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\workspace_masterarbeit\carsim_no_mlagents\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C215CD13-D874-4176-9482-AF5B5C9D6A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBEF6B3-4A31-4591-9E6E-1EE953B5E1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4DC23B-5923-4FA6-B608-7D9F8BF1AED5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
   <si>
     <t>Date</t>
   </si>
@@ -336,6 +336,24 @@
   </si>
   <si>
     <t>hard_standard distanceEvent_higherDistance100_ignoreCollisions</t>
+  </si>
+  <si>
+    <t>agent moved forwards</t>
+  </si>
+  <si>
+    <t>-rollout success_rate of 0.5 for medium tracks suggests a training with event_reward only is possible
+-however this result was obtained much slower than distanceRewardOnly</t>
+  </si>
+  <si>
+    <t>7h</t>
+  </si>
+  <si>
+    <t>distance and event reward incompatible together</t>
+  </si>
+  <si>
+    <t>-no learning progress
+-agent drives backwards
+-training was only executed for a relatively short time, however the distance reward alone results in quick learning in the same time</t>
   </si>
 </sst>
 </file>
@@ -698,10 +716,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C51CB6F-A2B2-448C-9258-B2680A9692D9}">
   <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1371,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -1365,6 +1383,12 @@
       </c>
       <c r="D10" t="s">
         <v>79</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="195" x14ac:dyDescent="0.25">
@@ -1720,7 +1744,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" ht="330" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1729,6 +1753,30 @@
       </c>
       <c r="C15" s="1">
         <v>45426</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="W15" t="s">
+        <v>36</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>103</v>
       </c>
       <c r="AD15" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
also log rollout difficulty proportions
</commit_message>
<xml_diff>
--- a/python/training_logs.xlsx
+++ b/python/training_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\workspace_masterarbeit\carsim_no_mlagents\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBEF6B3-4A31-4591-9E6E-1EE953B5E1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925DC996-67E0-45D1-94E8-74AC5E5D82EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4DC23B-5923-4FA6-B608-7D9F8BF1AED5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -354,6 +354,21 @@
     <t>-no learning progress
 -agent drives backwards
 -training was only executed for a relatively short time, however the distance reward alone results in quick learning in the same time</t>
+  </si>
+  <si>
+    <t>all_training_settings</t>
+  </si>
+  <si>
+    <t>randomEval</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>check if the training works when all tracks and lights are mixed together</t>
+  </si>
+  <si>
+    <t>it learns to complete the easy tracks only???</t>
   </si>
 </sst>
 </file>
@@ -714,12 +729,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C51CB6F-A2B2-448C-9258-B2680A9692D9}">
-  <dimension ref="A1:AD15"/>
+  <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,6 +1797,59 @@
         <v>98</v>
       </c>
     </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45427</v>
+      </c>
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>64</v>
+      </c>
+      <c r="K16">
+        <v>256</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more configs to execute
</commit_message>
<xml_diff>
--- a/python/training_logs.xlsx
+++ b/python/training_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\workspace_masterarbeit\carsim_no_mlagents\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ADCC1F-C348-4B1C-9E2A-B267601A2A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272994BF-7599-413C-914E-031179607A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4DC23B-5923-4FA6-B608-7D9F8BF1AED5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="125">
   <si>
     <t>Date</t>
   </si>
@@ -377,12 +377,50 @@
     <t>check if distance reward can solve easy tracks as well, as it sometimes learned to drive backwards before</t>
   </si>
   <si>
-    <t>- it learns to complete the easy and medium tracks, although not guaranteed
-- the random rollout track selection results in the success_rate and proportions of tracks of different difficulties to jump around a lot</t>
-  </si>
-  <si>
     <t>- do we need to fix the proportions of different difficulties?
 - do we need to simply increase the number of n_steps --&gt; number of rollout episodes</t>
+  </si>
+  <si>
+    <t>all_training_settings_more_nsteps</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>- it learns to complete the easy and medium tracks, although not guaranteed
+- the random rollout track selection results in the success_rate and proportions of tracks of different difficulties to jump around a lot
+- no succesful hard tracks</t>
+  </si>
+  <si>
+    <t>-no succesful hard tracks</t>
+  </si>
+  <si>
+    <t>-higher success rates for medium
+-more nsteps helps with learning</t>
+  </si>
+  <si>
+    <t>0.497</t>
+  </si>
+  <si>
+    <t>0.747</t>
+  </si>
+  <si>
+    <t>0.414</t>
+  </si>
+  <si>
+    <t>-completes easy tracks reliably
+-completes medium tracks in about 50%
+-fails on hard tracks (understandably)
+-light setting has only a minor influence on the success_rate (altough it was trained on standard only)</t>
+  </si>
+  <si>
+    <t>medium_standard_distance_reward_only_20.05.2024</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>currently running</t>
   </si>
 </sst>
 </file>
@@ -743,12 +781,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C51CB6F-A2B2-448C-9258-B2680A9692D9}">
-  <dimension ref="A1:AD17"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1850,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -1859,16 +1897,16 @@
         <v>36</v>
       </c>
       <c r="AB16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC16" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="AD16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -1878,6 +1916,9 @@
       <c r="C17" s="1">
         <v>45428</v>
       </c>
+      <c r="D17" t="s">
+        <v>114</v>
+      </c>
       <c r="E17" t="s">
         <v>110</v>
       </c>
@@ -1899,6 +1940,18 @@
       <c r="K17">
         <v>256</v>
       </c>
+      <c r="L17">
+        <v>800000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17">
+        <v>2048</v>
+      </c>
       <c r="P17" t="s">
         <v>33</v>
       </c>
@@ -1920,8 +1973,111 @@
       <c r="W17" t="s">
         <v>36</v>
       </c>
+      <c r="X17" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="AD17" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45429</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>64</v>
+      </c>
+      <c r="K18">
+        <v>1024</v>
+      </c>
+      <c r="L18">
+        <v>4700000</v>
+      </c>
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18">
+        <v>2048</v>
+      </c>
+      <c r="P18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>34</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18" t="s">
+        <v>36</v>
+      </c>
+      <c r="X18" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new config hard with freshObs
</commit_message>
<xml_diff>
--- a/python/training_logs.xlsx
+++ b/python/training_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\workspace_masterarbeit\carsim_no_mlagents\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272994BF-7599-413C-914E-031179607A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E6C84-5228-4DA5-9575-F389250A8AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A4DC23B-5923-4FA6-B608-7D9F8BF1AED5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{0A4DC23B-5923-4FA6-B608-7D9F8BF1AED5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="126">
   <si>
     <t>Date</t>
   </si>
@@ -392,13 +392,6 @@
 - no succesful hard tracks</t>
   </si>
   <si>
-    <t>-no succesful hard tracks</t>
-  </si>
-  <si>
-    <t>-higher success rates for medium
--more nsteps helps with learning</t>
-  </si>
-  <si>
     <t>0.497</t>
   </si>
   <si>
@@ -414,13 +407,25 @@
 -light setting has only a minor influence on the success_rate (altough it was trained on standard only)</t>
   </si>
   <si>
-    <t>medium_standard_distance_reward_only_20.05.2024</t>
-  </si>
-  <si>
     <t>3 days</t>
   </si>
   <si>
-    <t>currently running</t>
+    <t>medium_distance_reward_only_20.05.2024</t>
+  </si>
+  <si>
+    <t>-higher success rates for medium
+-more nsteps helps with learning
+-distance reward alone does not result in the agent wanting to finish episodes</t>
+  </si>
+  <si>
+    <t>0.629</t>
+  </si>
+  <si>
+    <t>0.887</t>
+  </si>
+  <si>
+    <t>-no succesful hard tracks
+-agent completed all goals but did not move to touch the finishLine in the medium setting for 10% of runs</t>
   </si>
 </sst>
 </file>
@@ -783,10 +788,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C51CB6F-A2B2-448C-9258-B2680A9692D9}">
   <dimension ref="A1:AD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="X21" sqref="X21"/>
+      <selection pane="bottomLeft" activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1974,25 +1979,25 @@
         <v>36</v>
       </c>
       <c r="X17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Y17" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>118</v>
-      </c>
-      <c r="AA17">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="AD17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -2003,7 +2008,7 @@
         <v>45429</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E18" t="s">
         <v>106</v>
@@ -2060,18 +2065,27 @@
         <v>36</v>
       </c>
       <c r="X18" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="s">
         <v>124</v>
       </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
       <c r="AB18" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>

</xml_diff>